<commit_message>
Column names revised (only change)
</commit_message>
<xml_diff>
--- a/4_ExpC_Vocab/Analysis/data/edited_dat/20230313_dat_target_start_to_demographic.xlsx
+++ b/4_ExpC_Vocab/Analysis/data/edited_dat/20230313_dat_target_start_to_demographic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ryunosuke/Dropbox/比喩関連/基盤数/SemanticSimilarityTest/code/experiment/2_ExpA_SST/OnlineExp/_data/edited_dat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryunosuke/Dropbox/比喩関連/基盤数/SemanticSimilarityTest/github/Japanese_version_of_SST/4_ExpC_Vocab/Analysis/data/edited_dat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DCCACC0-08F7-AE41-BB53-B6A703E3A301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E370BB16-7CFE-4A4F-B29F-2D8C3E964D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4920" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3920" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -1102,10 +1102,11 @@
     <t>AcademicDegree</t>
   </si>
   <si>
-    <t>CrowdworksID</t>
-  </si>
-  <si>
     <t>Q_PopulateResponse</t>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
@@ -1462,13 +1463,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="X7" sqref="X7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:28" ht="17">
+    <row r="1" spans="1:28">
       <c r="A1" s="3" t="s">
         <v>335</v>
       </c>
@@ -1545,14 +1546,14 @@
         <v>359</v>
       </c>
       <c r="Z1" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="AA1" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="AA1" s="3" t="s">
-        <v>361</v>
-      </c>
       <c r="AB1" s="2"/>
     </row>
-    <row r="2" spans="1:28" ht="17">
+    <row r="2" spans="1:28">
       <c r="A2" s="1">
         <v>44965.504687499997</v>
       </c>
@@ -1627,7 +1628,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="17">
+    <row r="3" spans="1:28">
       <c r="A3" s="1">
         <v>44965.5055208333</v>
       </c>
@@ -1702,7 +1703,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="17">
+    <row r="4" spans="1:28">
       <c r="A4" s="1">
         <v>44965.510474536997</v>
       </c>
@@ -1777,7 +1778,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="17">
+    <row r="5" spans="1:28">
       <c r="A5" s="1">
         <v>44965.510983796303</v>
       </c>
@@ -1852,7 +1853,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="17">
+    <row r="6" spans="1:28">
       <c r="A6" s="1">
         <v>44965.511018518497</v>
       </c>
@@ -1927,7 +1928,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="17">
+    <row r="7" spans="1:28">
       <c r="A7" s="1">
         <v>44965.511388888903</v>
       </c>
@@ -2002,7 +2003,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="17">
+    <row r="8" spans="1:28">
       <c r="A8" s="1">
         <v>44965.512407407397</v>
       </c>
@@ -2077,7 +2078,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="17">
+    <row r="9" spans="1:28">
       <c r="A9" s="1">
         <v>44965.514224537001</v>
       </c>
@@ -2152,7 +2153,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="17">
+    <row r="10" spans="1:28">
       <c r="A10" s="1">
         <v>44965.514120370397</v>
       </c>
@@ -2227,7 +2228,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="17">
+    <row r="11" spans="1:28">
       <c r="A11" s="1">
         <v>44965.515543981499</v>
       </c>
@@ -2302,7 +2303,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="17">
+    <row r="12" spans="1:28">
       <c r="A12" s="1">
         <v>44965.516469907401</v>
       </c>
@@ -2377,7 +2378,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="17">
+    <row r="13" spans="1:28">
       <c r="A13" s="1">
         <v>44965.516539351898</v>
       </c>
@@ -2452,7 +2453,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="17">
+    <row r="14" spans="1:28">
       <c r="A14" s="1">
         <v>44965.516655092601</v>
       </c>
@@ -2527,7 +2528,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="17">
+    <row r="15" spans="1:28">
       <c r="A15" s="1">
         <v>44965.517002314802</v>
       </c>
@@ -2602,7 +2603,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="17">
+    <row r="16" spans="1:28">
       <c r="A16" s="1">
         <v>44965.5168865741</v>
       </c>
@@ -2677,7 +2678,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="17">
+    <row r="17" spans="1:27">
       <c r="A17" s="1">
         <v>44965.5169328704</v>
       </c>
@@ -2752,7 +2753,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:27" ht="17">
+    <row r="18" spans="1:27">
       <c r="A18" s="1">
         <v>44965.5168402778</v>
       </c>
@@ -2827,7 +2828,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:27" ht="17">
+    <row r="19" spans="1:27">
       <c r="A19" s="1">
         <v>44965.5169328704</v>
       </c>
@@ -2902,7 +2903,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="17">
+    <row r="20" spans="1:27">
       <c r="A20" s="1">
         <v>44965.517060185201</v>
       </c>
@@ -2977,7 +2978,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:27" ht="17">
+    <row r="21" spans="1:27">
       <c r="A21" s="1">
         <v>44965.516574074099</v>
       </c>
@@ -3052,7 +3053,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="17">
+    <row r="22" spans="1:27">
       <c r="A22" s="1">
         <v>44965.517280092601</v>
       </c>
@@ -3127,7 +3128,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:27" ht="17">
+    <row r="23" spans="1:27">
       <c r="A23" s="1">
         <v>44965.5172916667</v>
       </c>
@@ -3202,7 +3203,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:27" ht="17">
+    <row r="24" spans="1:27">
       <c r="A24" s="1">
         <v>44965.516863425903</v>
       </c>
@@ -3277,7 +3278,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:27" ht="17">
+    <row r="25" spans="1:27">
       <c r="A25" s="1">
         <v>44965.517812500002</v>
       </c>
@@ -3352,7 +3353,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:27" ht="17">
+    <row r="26" spans="1:27">
       <c r="A26" s="1">
         <v>44965.516550925902</v>
       </c>
@@ -3427,7 +3428,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:27" ht="17">
+    <row r="27" spans="1:27">
       <c r="A27" s="1">
         <v>44965.5177430556</v>
       </c>
@@ -3502,7 +3503,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:27" ht="17">
+    <row r="28" spans="1:27">
       <c r="A28" s="1">
         <v>44965.5164814815</v>
       </c>
@@ -3577,7 +3578,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:27" ht="17">
+    <row r="29" spans="1:27">
       <c r="A29" s="1">
         <v>44965.517175925903</v>
       </c>
@@ -3652,7 +3653,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:27" ht="17">
+    <row r="30" spans="1:27">
       <c r="A30" s="1">
         <v>44965.517337963</v>
       </c>
@@ -3727,7 +3728,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="31" spans="1:27" ht="17">
+    <row r="31" spans="1:27">
       <c r="A31" s="1">
         <v>44965.517893518503</v>
       </c>
@@ -3802,7 +3803,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="32" spans="1:27" ht="17">
+    <row r="32" spans="1:27">
       <c r="A32" s="1">
         <v>44965.517847222203</v>
       </c>
@@ -3877,7 +3878,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="1:27" ht="17">
+    <row r="33" spans="1:27">
       <c r="A33" s="1">
         <v>44965.518067129597</v>
       </c>
@@ -3952,7 +3953,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:27" ht="17">
+    <row r="34" spans="1:27">
       <c r="A34" s="1">
         <v>44965.517974536997</v>
       </c>
@@ -4027,7 +4028,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="35" spans="1:27" ht="17">
+    <row r="35" spans="1:27">
       <c r="A35" s="1">
         <v>44965.517708333296</v>
       </c>
@@ -4102,7 +4103,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:27" ht="17">
+    <row r="36" spans="1:27">
       <c r="A36" s="1">
         <v>44965.518310185202</v>
       </c>
@@ -4177,7 +4178,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="37" spans="1:27" ht="17">
+    <row r="37" spans="1:27">
       <c r="A37" s="1">
         <v>44965.518414351798</v>
       </c>
@@ -4252,7 +4253,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="38" spans="1:27" ht="17">
+    <row r="38" spans="1:27">
       <c r="A38" s="1">
         <v>44965.518298611103</v>
       </c>
@@ -4327,7 +4328,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="39" spans="1:27" ht="17">
+    <row r="39" spans="1:27">
       <c r="A39" s="1">
         <v>44965.518333333297</v>
       </c>
@@ -4402,7 +4403,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="40" spans="1:27" ht="17">
+    <row r="40" spans="1:27">
       <c r="A40" s="1">
         <v>44965.5183217593</v>
       </c>
@@ -4477,7 +4478,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="41" spans="1:27" ht="17">
+    <row r="41" spans="1:27">
       <c r="A41" s="1">
         <v>44965.518564814804</v>
       </c>
@@ -4552,7 +4553,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="42" spans="1:27" ht="17">
+    <row r="42" spans="1:27">
       <c r="A42" s="1">
         <v>44965.517731481501</v>
       </c>
@@ -4627,7 +4628,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="43" spans="1:27" ht="17">
+    <row r="43" spans="1:27">
       <c r="A43" s="1">
         <v>44965.517650463</v>
       </c>
@@ -4702,7 +4703,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="44" spans="1:27" ht="17">
+    <row r="44" spans="1:27">
       <c r="A44" s="1">
         <v>44965.518819444398</v>
       </c>
@@ -4777,7 +4778,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="45" spans="1:27" ht="17">
+    <row r="45" spans="1:27">
       <c r="A45" s="1">
         <v>44965.518703703703</v>
       </c>
@@ -4852,7 +4853,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="46" spans="1:27" ht="17">
+    <row r="46" spans="1:27">
       <c r="A46" s="1">
         <v>44965.518518518496</v>
       </c>
@@ -4927,7 +4928,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="47" spans="1:27" ht="17">
+    <row r="47" spans="1:27">
       <c r="A47" s="1">
         <v>44965.519027777802</v>
       </c>
@@ -5002,7 +5003,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="48" spans="1:27" ht="17">
+    <row r="48" spans="1:27">
       <c r="A48" s="1">
         <v>44965.519282407397</v>
       </c>
@@ -5077,7 +5078,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="49" spans="1:27" ht="17">
+    <row r="49" spans="1:27">
       <c r="A49" s="1">
         <v>44965.519236111097</v>
       </c>
@@ -5152,7 +5153,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="50" spans="1:27" ht="17">
+    <row r="50" spans="1:27">
       <c r="A50" s="1">
         <v>44965.519699074102</v>
       </c>
@@ -5227,7 +5228,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="51" spans="1:27" ht="17">
+    <row r="51" spans="1:27">
       <c r="A51" s="1">
         <v>44965.520821759303</v>
       </c>
@@ -5302,7 +5303,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="52" spans="1:27" ht="17">
+    <row r="52" spans="1:27">
       <c r="A52" s="1">
         <v>44965.520277777803</v>
       </c>
@@ -5377,7 +5378,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="53" spans="1:27" ht="17">
+    <row r="53" spans="1:27">
       <c r="A53" s="1">
         <v>44965.521099537</v>
       </c>
@@ -5452,7 +5453,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="54" spans="1:27" ht="17">
+    <row r="54" spans="1:27">
       <c r="A54" s="1">
         <v>44965.522430555597</v>
       </c>
@@ -5527,7 +5528,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="55" spans="1:27" ht="17">
+    <row r="55" spans="1:27">
       <c r="A55" s="1">
         <v>44965.5231712963</v>
       </c>
@@ -5602,7 +5603,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="56" spans="1:27" ht="17">
+    <row r="56" spans="1:27">
       <c r="A56" s="1">
         <v>44965.523449074099</v>
       </c>
@@ -5677,7 +5678,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="57" spans="1:27" ht="17">
+    <row r="57" spans="1:27">
       <c r="A57" s="1">
         <v>44965.524791666699</v>
       </c>
@@ -5752,7 +5753,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="58" spans="1:27" ht="17">
+    <row r="58" spans="1:27">
       <c r="A58" s="1">
         <v>44965.528495370403</v>
       </c>
@@ -5827,7 +5828,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="59" spans="1:27" ht="17">
+    <row r="59" spans="1:27">
       <c r="A59" s="1">
         <v>44965.531192129602</v>
       </c>
@@ -5902,7 +5903,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="60" spans="1:27" ht="17">
+    <row r="60" spans="1:27">
       <c r="A60" s="1">
         <v>44965.531944444403</v>
       </c>
@@ -5977,7 +5978,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="61" spans="1:27" ht="17">
+    <row r="61" spans="1:27">
       <c r="A61" s="1">
         <v>44965.534618055601</v>
       </c>
@@ -6052,7 +6053,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="62" spans="1:27" ht="17">
+    <row r="62" spans="1:27">
       <c r="A62" s="1">
         <v>44965.518576388902</v>
       </c>
@@ -6127,7 +6128,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="63" spans="1:27" ht="17">
+    <row r="63" spans="1:27">
       <c r="A63" s="1">
         <v>44965.545844907399</v>
       </c>
@@ -6202,7 +6203,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="64" spans="1:27" ht="17">
+    <row r="64" spans="1:27">
       <c r="A64" s="1">
         <v>44965.546238425901</v>
       </c>
@@ -6277,7 +6278,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="65" spans="1:27" ht="17">
+    <row r="65" spans="1:27">
       <c r="A65" s="1">
         <v>44965.548159722202</v>
       </c>
@@ -6352,7 +6353,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="66" spans="1:27" ht="17">
+    <row r="66" spans="1:27">
       <c r="A66" s="1">
         <v>44965.5480902778</v>
       </c>
@@ -6427,7 +6428,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="67" spans="1:27" ht="17">
+    <row r="67" spans="1:27">
       <c r="A67" s="1">
         <v>44965.548506944397</v>
       </c>
@@ -6502,7 +6503,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="68" spans="1:27" ht="17">
+    <row r="68" spans="1:27">
       <c r="A68" s="1">
         <v>44965.550659722197</v>
       </c>
@@ -6577,7 +6578,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="69" spans="1:27" ht="17">
+    <row r="69" spans="1:27">
       <c r="A69" s="1">
         <v>44965.551446759302</v>
       </c>
@@ -6652,7 +6653,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="70" spans="1:27" ht="17">
+    <row r="70" spans="1:27">
       <c r="A70" s="1">
         <v>44965.557256944398</v>
       </c>
@@ -6727,7 +6728,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="71" spans="1:27" ht="17">
+    <row r="71" spans="1:27">
       <c r="A71" s="1">
         <v>44965.557337963</v>
       </c>
@@ -6802,7 +6803,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="72" spans="1:27" ht="17">
+    <row r="72" spans="1:27">
       <c r="A72" s="1">
         <v>44965.558229166701</v>
       </c>
@@ -6877,7 +6878,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="73" spans="1:27" ht="17">
+    <row r="73" spans="1:27">
       <c r="A73" s="1">
         <v>44965.558321759301</v>
       </c>
@@ -6952,7 +6953,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="74" spans="1:27" ht="17">
+    <row r="74" spans="1:27">
       <c r="A74" s="1">
         <v>44965.558356481502</v>
       </c>
@@ -7027,7 +7028,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="75" spans="1:27" ht="17">
+    <row r="75" spans="1:27">
       <c r="A75" s="1">
         <v>44965.558229166701</v>
       </c>
@@ -7102,7 +7103,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="76" spans="1:27" ht="17">
+    <row r="76" spans="1:27">
       <c r="A76" s="1">
         <v>44965.558495370402</v>
       </c>
@@ -7177,7 +7178,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="77" spans="1:27" ht="17">
+    <row r="77" spans="1:27">
       <c r="A77" s="1">
         <v>44965.558414351799</v>
       </c>
@@ -7252,7 +7253,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="78" spans="1:27" ht="17">
+    <row r="78" spans="1:27">
       <c r="A78" s="1">
         <v>44965.558101851799</v>
       </c>
@@ -7327,7 +7328,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="79" spans="1:27" ht="17">
+    <row r="79" spans="1:27">
       <c r="A79" s="1">
         <v>44965.558553240699</v>
       </c>
@@ -7402,7 +7403,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="80" spans="1:27" ht="17">
+    <row r="80" spans="1:27">
       <c r="A80" s="1">
         <v>44965.558738425898</v>
       </c>
@@ -7477,7 +7478,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="81" spans="1:27" ht="17">
+    <row r="81" spans="1:27">
       <c r="A81" s="1">
         <v>44965.558784722198</v>
       </c>
@@ -7552,7 +7553,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="82" spans="1:27" ht="17">
+    <row r="82" spans="1:27">
       <c r="A82" s="1">
         <v>44965.558379629598</v>
       </c>
@@ -7627,7 +7628,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="83" spans="1:27" ht="17">
+    <row r="83" spans="1:27">
       <c r="A83" s="1">
         <v>44965.559560185196</v>
       </c>
@@ -7702,7 +7703,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="84" spans="1:27" ht="17">
+    <row r="84" spans="1:27">
       <c r="A84" s="1">
         <v>44965.559351851902</v>
       </c>
@@ -7777,7 +7778,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="85" spans="1:27" ht="17">
+    <row r="85" spans="1:27">
       <c r="A85" s="1">
         <v>44965.559722222199</v>
       </c>
@@ -7852,7 +7853,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="86" spans="1:27" ht="17">
+    <row r="86" spans="1:27">
       <c r="A86" s="1">
         <v>44965.559537036999</v>
       </c>
@@ -7927,7 +7928,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="87" spans="1:27" ht="17">
+    <row r="87" spans="1:27">
       <c r="A87" s="1">
         <v>44965.560370370396</v>
       </c>
@@ -8002,7 +8003,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="88" spans="1:27" ht="17">
+    <row r="88" spans="1:27">
       <c r="A88" s="1">
         <v>44965.561134259297</v>
       </c>
@@ -8077,7 +8078,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="89" spans="1:27" ht="17">
+    <row r="89" spans="1:27">
       <c r="A89" s="1">
         <v>44965.561041666697</v>
       </c>
@@ -8152,7 +8153,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="90" spans="1:27" ht="17">
+    <row r="90" spans="1:27">
       <c r="A90" s="1">
         <v>44965.560034722199</v>
       </c>
@@ -8227,7 +8228,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="91" spans="1:27" ht="17">
+    <row r="91" spans="1:27">
       <c r="A91" s="1">
         <v>44965.563599537003</v>
       </c>
@@ -8302,7 +8303,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="92" spans="1:27" ht="17">
+    <row r="92" spans="1:27">
       <c r="A92" s="1">
         <v>44965.564918981501</v>
       </c>
@@ -8377,7 +8378,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="93" spans="1:27" ht="17">
+    <row r="93" spans="1:27">
       <c r="A93" s="1">
         <v>44965.518194444398</v>
       </c>
@@ -8452,7 +8453,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="94" spans="1:27" ht="17">
+    <row r="94" spans="1:27">
       <c r="A94" s="1">
         <v>44965.579050925902</v>
       </c>
@@ -8527,7 +8528,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="95" spans="1:27" ht="17">
+    <row r="95" spans="1:27">
       <c r="A95" s="1">
         <v>44965.600312499999</v>
       </c>
@@ -8602,7 +8603,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="96" spans="1:27" ht="17">
+    <row r="96" spans="1:27">
       <c r="A96" s="1">
         <v>44965.601678240702</v>
       </c>
@@ -8677,7 +8678,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="97" spans="1:27" ht="17">
+    <row r="97" spans="1:27">
       <c r="A97" s="1">
         <v>44965.602002314801</v>
       </c>
@@ -8752,7 +8753,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="98" spans="1:27" ht="17">
+    <row r="98" spans="1:27">
       <c r="A98" s="1">
         <v>44965.643020833297</v>
       </c>
@@ -8827,7 +8828,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="99" spans="1:27" ht="17">
+    <row r="99" spans="1:27">
       <c r="A99" s="1">
         <v>44965.766041666699</v>
       </c>
@@ -8902,7 +8903,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="100" spans="1:27" ht="17">
+    <row r="100" spans="1:27">
       <c r="A100" s="1">
         <v>44965.870682870402</v>
       </c>
@@ -8977,7 +8978,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="101" spans="1:27" ht="17">
+    <row r="101" spans="1:27">
       <c r="A101" s="1">
         <v>44966.380011574103</v>
       </c>

</xml_diff>